<commit_message>
Font fallback. Using fusion cache.
</commit_message>
<xml_diff>
--- a/FRJ.Tools.SimpleWorkSheet.Examples/Output/001_HelloWorld.xlsx
+++ b/FRJ.Tools.SimpleWorkSheet.Examples/Output/001_HelloWorld.xlsx
@@ -5,7 +5,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HelloWorld" sheetId="1" r:id="R28482b48376a4dc2"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HelloWorld" sheetId="1" r:id="Rba673db480864f8e"/>
   </x:sheets>
   <x:calcPr fullCalcOnLoad="1"/>
 </x:workbook>
@@ -29,7 +29,7 @@
     <x:font>
       <x:sz val="12"/>
       <x:color rgb="FF000000"/>
-      <x:name val="Aptos Narrow"/>
+      <x:name val="Arial"/>
     </x:font>
   </x:fonts>
   <x:fills count="2">

</xml_diff>